<commit_message>
Excel file containing the ANOVA results of the main results.
</commit_message>
<xml_diff>
--- a/Output/Anova tables mericarp bioclimate.xlsx
+++ b/Output/Anova tables mericarp bioclimate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Vault of Ideas\20 - 29 Tribulus Research\22 Chapter. Tribulus phenotypic variation in mainland and island populations\22.03 R code\Tribulus-mericarp-morphology\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A0BE89-AA50-4BB6-B1B8-C9095D6CC231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D416BF24-C179-40B2-82B2-18D4C888780E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="2430" windowWidth="21600" windowHeight="11400" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="35">
   <si>
     <t xml:space="preserve">Trait </t>
   </si>
@@ -83,13 +83,125 @@
   </si>
   <si>
     <t>Lower spines</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A) Mericarp – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island</t>
+    </r>
+  </si>
+  <si>
+    <t>Trait</t>
+  </si>
+  <si>
+    <t>Continental/Island</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <r>
+      <t>χ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Spine tip distance</t>
+  </si>
+  <si>
+    <t>Mericarp Size (PC1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B) Flowers – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island</t>
+    </r>
+  </si>
+  <si>
+    <t>Petal length</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C) Flowers – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Galápagos vs other islands</t>
+    </r>
+  </si>
+  <si>
+    <t>Galápagos/Other islands</t>
+  </si>
+  <si>
+    <t>Bio1</t>
+  </si>
+  <si>
+    <t>Bio4</t>
+  </si>
+  <si>
+    <t>Bio12</t>
+  </si>
+  <si>
+    <t>Bio15</t>
+  </si>
+  <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Herbarium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +225,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -122,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -157,37 +311,197 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC27BD51-B649-4FE2-8231-40ED64EB6F14}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,409 +828,1375 @@
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="F1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="W1" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="23"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="23"/>
+    </row>
+    <row r="3" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>0.74480000000000002</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>0.3881348</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="F3" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" s="25"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB3" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD3" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>11.7987</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>5.9270000000000004E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="44">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="I4" s="44">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J4" s="45">
+        <v>5.6459999999999999</v>
+      </c>
+      <c r="K4" s="45">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="L4" s="44">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M4" s="44">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="N4" s="44">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="O4" s="44">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="P4" s="45">
+        <v>4.3730000000000002</v>
+      </c>
+      <c r="Q4" s="45">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="R4" s="44">
+        <v>2.2519999999999998</v>
+      </c>
+      <c r="S4" s="44">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="T4" s="44">
+        <v>3.097</v>
+      </c>
+      <c r="U4" s="44">
+        <v>7.8E-2</v>
+      </c>
+      <c r="W4" s="25"/>
+      <c r="X4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y4" s="22">
+        <v>14.138999999999999</v>
+      </c>
+      <c r="Z4" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="22">
+        <v>6.1760000000000002</v>
+      </c>
+      <c r="AB4" s="22">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AC4" s="21">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>0.1202</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>0.72884590000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="44">
+        <v>2.202</v>
+      </c>
+      <c r="I5" s="44">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="J5" s="44">
+        <v>2.8290000000000002</v>
+      </c>
+      <c r="K5" s="44">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="L5" s="44">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="M5" s="44">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="N5" s="44">
+        <v>0.214</v>
+      </c>
+      <c r="O5" s="44">
+        <v>0.64300000000000002</v>
+      </c>
+      <c r="P5" s="44">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="Q5" s="44">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="R5" s="44">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="S5" s="46">
+        <v>0.78</v>
+      </c>
+      <c r="T5" s="44">
+        <v>2.5470000000000002</v>
+      </c>
+      <c r="U5" s="46">
+        <v>0.11</v>
+      </c>
+      <c r="W5" s="25"/>
+      <c r="X5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y5" s="22">
+        <v>12.047000000000001</v>
+      </c>
+      <c r="Z5" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA5" s="21">
+        <v>3.2280000000000002</v>
+      </c>
+      <c r="AB5" s="21">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>1.2E-2</v>
+      </c>
+      <c r="AD5" s="36">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>5.625</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>1.7706300000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="F6" s="26"/>
+      <c r="G6" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="45">
+        <v>5.6689999999999996</v>
+      </c>
+      <c r="I6" s="45">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J6" s="45">
+        <v>11.401999999999999</v>
+      </c>
+      <c r="K6" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="48">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="M6" s="48">
+        <v>0.443</v>
+      </c>
+      <c r="N6" s="44">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="O6" s="44">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="P6" s="44">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="R6" s="44">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="S6" s="44">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="T6" s="45">
+        <v>6.8789999999999996</v>
+      </c>
+      <c r="U6" s="45">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="W6" s="25"/>
+      <c r="X6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>51.506</v>
+      </c>
+      <c r="Z6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA6" s="22">
+        <v>11.106999999999999</v>
+      </c>
+      <c r="AB6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC6" s="21">
+        <v>0.309</v>
+      </c>
+      <c r="AD6" s="21">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>2.5206</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>0.11236939999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9" t="s">
+      <c r="F7" s="26"/>
+      <c r="G7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="44">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="I7" s="44">
+        <v>0.439</v>
+      </c>
+      <c r="J7" s="44">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="K7" s="44">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="L7" s="44">
+        <v>0.495</v>
+      </c>
+      <c r="M7" s="44">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="N7" s="44">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="O7" s="44">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="P7" s="44">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="Q7" s="44">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="R7" s="44">
+        <v>1.5620000000000001</v>
+      </c>
+      <c r="S7" s="44">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="T7" s="44">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="U7" s="44">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="W7" s="25"/>
+      <c r="X7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y7" s="40">
+        <v>5.85</v>
+      </c>
+      <c r="Z7" s="22">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AA7" s="21">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="AB7" s="21">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>1.077</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="5">
         <v>2.6347</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>0.1045527</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="F8" s="26"/>
+      <c r="G8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="49">
+        <v>1.53</v>
+      </c>
+      <c r="I8" s="50">
+        <v>0.216</v>
+      </c>
+      <c r="J8" s="50">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="K8" s="50">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="L8" s="50">
+        <v>1E-3</v>
+      </c>
+      <c r="M8" s="49">
+        <v>0.97</v>
+      </c>
+      <c r="N8" s="51">
+        <v>8.6050000000000004</v>
+      </c>
+      <c r="O8" s="51">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P8" s="51">
+        <v>10.701000000000001</v>
+      </c>
+      <c r="Q8" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="R8" s="51">
+        <v>19.497</v>
+      </c>
+      <c r="S8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="T8" s="51">
+        <v>18.157</v>
+      </c>
+      <c r="U8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="W8" s="25"/>
+      <c r="X8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y8" s="38">
+        <v>77.921000000000006</v>
+      </c>
+      <c r="Z8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA8" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB8" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC8" s="37">
+        <v>3.254</v>
+      </c>
+      <c r="AD8" s="37">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="6">
         <v>2.2663000000000002</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="6">
         <v>0.13220000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="F9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="29"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
+    </row>
+    <row r="10" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>6.4333999999999998</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>1.12E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
+      <c r="F10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="W10" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>0.32250000000000001</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>0.57010000000000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="U11" s="23"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD11" s="23"/>
+    </row>
+    <row r="12" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>0.90780000000000005</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>0.3407</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="U12" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="12"/>
+      <c r="X12" s="39"/>
+      <c r="Y12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z12" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB12" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD12" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="3">
         <v>5.5100000000000003E-2</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>0.81440000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9" t="s">
+      <c r="F13" s="27"/>
+      <c r="G13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="52">
+        <v>10.042999999999999</v>
+      </c>
+      <c r="I13" s="52">
+        <v>1E-3</v>
+      </c>
+      <c r="J13" s="53">
+        <v>15.95</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="54">
+        <v>13.657</v>
+      </c>
+      <c r="O13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="P13" s="52">
+        <v>15.298999999999999</v>
+      </c>
+      <c r="Q13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" s="55">
+        <v>2.1669999999999998</v>
+      </c>
+      <c r="S13" s="56">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="T13" s="57">
+        <v>18.533000000000001</v>
+      </c>
+      <c r="U13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="W13" s="11"/>
+      <c r="X13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y13" s="21">
+        <v>1.3859999999999999</v>
+      </c>
+      <c r="Z13" s="21">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="AA13" s="22">
+        <v>15.622999999999999</v>
+      </c>
+      <c r="AB13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD13" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="5">
         <v>2.5390000000000001</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>0.1111</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="F14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="W14" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+    </row>
+    <row r="15" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="7">
         <v>6.1447000000000003</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="7">
         <v>1.3181E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
+      <c r="F15" s="28"/>
+      <c r="G15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="U15" s="14"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD15" s="23"/>
+    </row>
+    <row r="16" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>16.3093</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="8">
         <v>5.38E-5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
+      <c r="F16" s="28"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="T16" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="U16" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="W16" s="20"/>
+      <c r="X16" s="39"/>
+      <c r="Y16" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z16" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB16" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD16" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="16"/>
+      <c r="B17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="3">
         <v>0.10680000000000001</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="3">
         <v>0.74376299999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
+      <c r="F17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="59">
+        <v>84.867000000000004</v>
+      </c>
+      <c r="I17" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="59">
+        <v>5.1879999999999997</v>
+      </c>
+      <c r="K17" s="59">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="L17" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="60">
+        <v>1.909</v>
+      </c>
+      <c r="O17" s="60">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="P17" s="60">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="Q17" s="60">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="R17" s="60">
+        <v>2.6219999999999999</v>
+      </c>
+      <c r="S17" s="60">
+        <v>0.105</v>
+      </c>
+      <c r="T17" s="60">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="U17" s="61">
+        <v>0.47</v>
+      </c>
+      <c r="W17" s="25"/>
+      <c r="X17" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y17" s="42">
+        <v>157.14699999999999</v>
+      </c>
+      <c r="Z17" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA17" s="42">
+        <v>9.4529999999999994</v>
+      </c>
+      <c r="AB17" s="42">
+        <v>2E-3</v>
+      </c>
+      <c r="AC17" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD17" s="41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="3">
         <v>0.51959999999999995</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="3">
         <v>0.470995</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
+      <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="3">
         <v>0.57389999999999997</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="3">
         <v>0.44870100000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="1:30" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="9">
         <v>6.7979000000000003</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="9">
         <v>9.1269999999999997E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="6">
         <v>0.72799999999999998</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="6">
         <v>0.39350000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
+      <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="3">
         <v>0.25779999999999997</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="3">
         <v>0.61170000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="3">
         <v>0.42</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="3">
         <v>0.51690000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="3">
         <v>1.2594000000000001</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="3">
         <v>0.26179999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>1.8427</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="3">
         <v>0.17460000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9" t="s">
+    <row r="26" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="5">
         <v>8.1699999999999995E-2</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="5">
         <v>0.77510000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="6">
         <v>1.5370999999999999</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="6">
         <v>0.2150456</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="3">
         <v>1.2051000000000001</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="3">
         <v>0.27229569999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6" t="s">
+    <row r="29" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
+      <c r="B29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="4">
         <v>8.0871999999999993</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="4">
         <v>4.4578999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16"/>
+      <c r="B30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>12.2906</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>4.5530000000000001E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
+      <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="4">
         <v>19.7334</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="8">
         <v>8.9029999999999993E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9" t="s">
+    <row r="32" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="9">
         <v>17.956399999999999</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="10">
         <v>2.26E-5</v>
       </c>
     </row>
+    <row r="33" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A8"/>
+  <mergeCells count="42">
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="W10:AD10"/>
+    <mergeCell ref="W14:AD14"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="AC11:AD11"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="A21:A26"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="F1:U1"/>
     <mergeCell ref="A27:A32"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="F10:U10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="F14:U14"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the results of mainland_ohter ANOVA
</commit_message>
<xml_diff>
--- a/Output/Anova tables mericarp bioclimate.xlsx
+++ b/Output/Anova tables mericarp bioclimate.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Vault of Ideas\20 - 29 Tribulus Research\22 Chapter. Tribulus phenotypic variation in mainland and island populations\22.03 R code\Tribulus-mericarp-morphology\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0D0B29-11C2-4DD4-8731-D0266063ECF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF191A6-49B6-4464-AE0E-1C76F6AE2430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual dataset" sheetId="1" r:id="rId1"/>
     <sheet name="Mean Datasets" sheetId="2" r:id="rId2"/>
+    <sheet name="Removed Galapagos Summary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="28">
   <si>
     <t>P</t>
   </si>
@@ -177,14 +178,91 @@
       <t>continental vs island</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Continental/Island </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A) Mericarp – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Galápagos removed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B) Flowers – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Galápagos removed</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -295,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -306,167 +384,149 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC27BD51-B649-4FE2-8231-40ED64EB6F14}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,1002 +860,1002 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="R1" s="15" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="R1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="42"/>
+      <c r="M2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="R2" s="11"/>
+      <c r="P2" s="42"/>
+      <c r="R2" s="1"/>
       <c r="S2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8" t="s">
+      <c r="U2" s="42"/>
+      <c r="V2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8" t="s">
+      <c r="W2" s="42"/>
+      <c r="X2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="8"/>
+      <c r="Y2" s="42"/>
     </row>
     <row r="3" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="W3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="24" t="s">
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="21">
         <v>0.66400000000000003</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="21">
         <v>0.41399999999999998</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="22">
         <v>5.6459999999999999</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="22">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="21">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="21">
         <v>0.93700000000000006</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="21">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="21">
         <v>0.79400000000000004</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="22">
         <v>4.3730000000000002</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="22">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="21">
         <v>2.2519999999999998</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="21">
         <v>0.13300000000000001</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="21">
         <v>3.097</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="21">
         <v>7.8E-2</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="5">
         <v>14.138999999999999</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="5">
         <v>6.1760000000000002</v>
       </c>
-      <c r="W4" s="7">
+      <c r="W4" s="5">
         <v>1.2E-2</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="4">
         <v>0.48899999999999999</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="4">
         <v>0.48399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="21">
         <v>2.202</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="21">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="21">
         <v>2.8290000000000002</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="21">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="21">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="21">
         <v>0.86499999999999999</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="21">
         <v>0.214</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="21">
         <v>0.64300000000000002</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="21">
         <v>0.84499999999999997</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="21">
         <v>0.35699999999999998</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="21">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="23">
         <v>0.78</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="21">
         <v>2.5470000000000002</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="23">
         <v>0.11</v>
       </c>
-      <c r="R5" s="11"/>
+      <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="5">
         <v>12.047000000000001</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="4">
         <v>3.2280000000000002</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="4">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="4">
         <v>1.2E-2</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="12">
         <v>0.91</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="22">
         <v>5.6689999999999996</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="22">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="22">
         <v>11.401999999999999</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="21">
         <v>0.58599999999999997</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="21">
         <v>0.443</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="21">
         <v>0.13200000000000001</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="21">
         <v>0.71599999999999997</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="21">
         <v>0.11899999999999999</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="21">
         <v>0.72899999999999998</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="21">
         <v>0.46600000000000003</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="21">
         <v>0.49399999999999999</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="22">
         <v>6.8789999999999996</v>
       </c>
-      <c r="P6" s="31">
+      <c r="P6" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="R6" s="11"/>
+      <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="5">
         <v>51.506</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="U6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="5">
         <v>11.106999999999999</v>
       </c>
-      <c r="W6" s="7" t="s">
+      <c r="W6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="4">
         <v>0.309</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y6" s="4">
         <v>0.57799999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="21">
         <v>0.59699999999999998</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="21">
         <v>0.439</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="21">
         <v>0.59699999999999998</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="21">
         <v>0.40799999999999997</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="21">
         <v>0.495</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="21">
         <v>0.48099999999999998</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="21">
         <v>0.56299999999999994</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="21">
         <v>0.45300000000000001</v>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="21">
         <v>0.55300000000000005</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="21">
         <v>0.45600000000000002</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="21">
         <v>1.5620000000000001</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="21">
         <v>0.21099999999999999</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="21">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="21">
         <v>0.82399999999999995</v>
       </c>
-      <c r="R7" s="11"/>
+      <c r="R7" s="1"/>
       <c r="S7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="25">
+      <c r="T7" s="16">
         <v>5.85</v>
       </c>
-      <c r="U7" s="7">
+      <c r="U7" s="5">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="V7" s="6">
+      <c r="V7" s="4">
         <v>0.73099999999999998</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7" s="4">
         <v>0.39200000000000002</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7" s="4">
         <v>1.077</v>
       </c>
-      <c r="Y7" s="6">
+      <c r="Y7" s="4">
         <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="25">
         <v>1.53</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="26">
         <v>0.216</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="26">
         <v>0.57899999999999996</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="26">
         <v>0.44600000000000001</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="26">
         <v>1E-3</v>
       </c>
-      <c r="H8" s="35">
+      <c r="H8" s="25">
         <v>0.97</v>
       </c>
-      <c r="I8" s="37">
+      <c r="I8" s="27">
         <v>8.6050000000000004</v>
       </c>
-      <c r="J8" s="37">
+      <c r="J8" s="27">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="K8" s="37">
+      <c r="K8" s="27">
         <v>10.701000000000001</v>
       </c>
-      <c r="L8" s="37">
+      <c r="L8" s="27">
         <v>1E-3</v>
       </c>
-      <c r="M8" s="37">
+      <c r="M8" s="27">
         <v>19.497</v>
       </c>
-      <c r="N8" s="23" t="s">
+      <c r="N8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="37">
+      <c r="O8" s="27">
         <v>18.157</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="19" t="s">
+      <c r="R8" s="1"/>
+      <c r="S8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="T8" s="23">
+      <c r="T8" s="14">
         <v>77.921000000000006</v>
       </c>
-      <c r="U8" s="23" t="s">
+      <c r="U8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="22" t="s">
+      <c r="V8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="W8" s="22" t="s">
+      <c r="W8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="X8" s="22">
+      <c r="X8" s="13">
         <v>3.254</v>
       </c>
-      <c r="Y8" s="22">
+      <c r="Y8" s="13">
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="4">
         <v>1.4870000000000001</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="4">
         <v>0.222</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="5">
         <v>7.3840000000000003</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="4">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="4">
         <v>0.79500000000000004</v>
       </c>
-      <c r="I9" s="44">
+      <c r="I9" s="21">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="J9" s="44">
+      <c r="J9" s="21">
         <v>0.83599999999999997</v>
       </c>
-      <c r="K9" s="44">
+      <c r="K9" s="21">
         <v>1.9410000000000001</v>
       </c>
-      <c r="L9" s="44">
+      <c r="L9" s="21">
         <v>0.16300000000000001</v>
       </c>
-      <c r="M9" s="44">
+      <c r="M9" s="21">
         <v>2.3450000000000002</v>
       </c>
-      <c r="N9" s="44">
+      <c r="N9" s="21">
         <v>0.125</v>
       </c>
-      <c r="O9" s="52">
+      <c r="O9" s="21">
         <v>2.9340000000000002</v>
       </c>
-      <c r="P9" s="57">
+      <c r="P9" s="36">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11" t="s">
+      <c r="R9" s="1"/>
+      <c r="S9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T9" s="10">
+      <c r="T9" s="5">
         <v>24.992000000000001</v>
       </c>
-      <c r="U9" s="7" t="s">
+      <c r="U9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V9" s="10">
+      <c r="V9" s="5">
         <v>7.298</v>
       </c>
-      <c r="W9" s="10">
+      <c r="W9" s="5">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="X9" s="9">
+      <c r="X9" s="4">
         <v>0.19800000000000001</v>
       </c>
-      <c r="Y9" s="9">
+      <c r="Y9" s="4">
         <v>0.65500000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="R10" s="15" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="R10" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="42"/>
+      <c r="E11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="42"/>
+      <c r="G11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8" t="s">
+      <c r="H11" s="42"/>
+      <c r="I11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8" t="s">
+      <c r="J11" s="42"/>
+      <c r="K11" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8" t="s">
+      <c r="L11" s="42"/>
+      <c r="M11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="42"/>
+      <c r="O11" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="8"/>
+      <c r="P11" s="42"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="8" t="s">
+      <c r="S11" s="5"/>
+      <c r="T11" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8" t="s">
+      <c r="U11" s="42"/>
+      <c r="V11" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8" t="s">
+      <c r="W11" s="42"/>
+      <c r="X11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="Y11" s="8"/>
+      <c r="Y11" s="42"/>
     </row>
     <row r="12" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="17" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="R12" s="2"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="U12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="W12" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X12" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y12" s="24" t="s">
+      <c r="S12" s="15"/>
+      <c r="T12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="28">
         <v>10.042999999999999</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="28">
         <v>1E-3</v>
       </c>
-      <c r="E13" s="39">
+      <c r="E13" s="29">
         <v>15.95</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="28">
         <v>13.657</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K13" s="38">
+      <c r="K13" s="28">
         <v>15.298999999999999</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M13" s="41">
+      <c r="M13" s="30">
         <v>2.1669999999999998</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13" s="31">
         <v>0.14000000000000001</v>
       </c>
-      <c r="O13" s="43">
+      <c r="O13" s="28">
         <v>18.533000000000001</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="P13" s="5" t="s">
         <v>21</v>
       </c>
       <c r="R13" s="1"/>
-      <c r="S13" s="6" t="s">
+      <c r="S13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="6">
+      <c r="T13" s="4">
         <v>1.3859999999999999</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="4">
         <v>0.23899999999999999</v>
       </c>
-      <c r="V13" s="7">
+      <c r="V13" s="5">
         <v>15.622999999999999</v>
       </c>
-      <c r="W13" s="10" t="s">
+      <c r="W13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X13" s="6" t="s">
+      <c r="X13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y13" s="6" t="s">
+      <c r="Y13" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="R14" s="15" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="R14" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
     </row>
     <row r="15" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
+      <c r="D15" s="44"/>
+      <c r="E15" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4" t="s">
+      <c r="F15" s="44"/>
+      <c r="G15" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4" t="s">
+      <c r="H15" s="44"/>
+      <c r="I15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4" t="s">
+      <c r="J15" s="44"/>
+      <c r="K15" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4" t="s">
+      <c r="L15" s="44"/>
+      <c r="M15" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="N15" s="44"/>
+      <c r="O15" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="4"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="8" t="s">
+      <c r="P15" s="44"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8" t="s">
+      <c r="U15" s="42"/>
+      <c r="V15" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8" t="s">
+      <c r="W15" s="42"/>
+      <c r="X15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="Y15" s="8"/>
+      <c r="Y15" s="42"/>
     </row>
     <row r="16" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P16" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R16" s="5"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="U16" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="W16" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y16" s="24" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" s="2"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="U16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W16" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y16" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="45">
+      <c r="C17" s="32">
         <v>84.867000000000004</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="45">
+      <c r="E17" s="32">
         <v>5.1879999999999997</v>
       </c>
-      <c r="F17" s="45">
+      <c r="F17" s="32">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="33">
         <v>1.909</v>
       </c>
-      <c r="J17" s="46">
+      <c r="J17" s="33">
         <v>0.16700000000000001</v>
       </c>
-      <c r="K17" s="46">
+      <c r="K17" s="33">
         <v>0.47099999999999997</v>
       </c>
-      <c r="L17" s="46">
+      <c r="L17" s="33">
         <v>0.49199999999999999</v>
       </c>
-      <c r="M17" s="46">
+      <c r="M17" s="33">
         <v>2.6219999999999999</v>
       </c>
-      <c r="N17" s="46">
+      <c r="N17" s="33">
         <v>0.105</v>
       </c>
-      <c r="O17" s="46">
+      <c r="O17" s="33">
         <v>0.52200000000000002</v>
       </c>
-      <c r="P17" s="47">
+      <c r="P17" s="34">
         <v>0.47</v>
       </c>
-      <c r="R17" s="11"/>
-      <c r="S17" s="27" t="s">
+      <c r="R17" s="1"/>
+      <c r="S17" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="T17" s="28">
+      <c r="T17" s="19">
         <v>157.14699999999999</v>
       </c>
-      <c r="U17" s="23" t="s">
+      <c r="U17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V17" s="28">
+      <c r="V17" s="19">
         <v>9.4529999999999994</v>
       </c>
-      <c r="W17" s="28">
+      <c r="W17" s="19">
         <v>2E-3</v>
       </c>
-      <c r="X17" s="27" t="s">
+      <c r="X17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="Y17" s="27" t="s">
+      <c r="Y17" s="18" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1807,18 +1867,14 @@
     <row r="34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="X15:Y15"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="R10:Y10"/>
-    <mergeCell ref="R14:Y14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="V15:W15"/>
-    <mergeCell ref="X2:Y2"/>
-    <mergeCell ref="T11:U11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G15:H15"/>
@@ -1835,14 +1891,18 @@
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="A14:P14"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="X15:Y15"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="R10:Y10"/>
+    <mergeCell ref="R14:Y14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="V15:W15"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="T2:U2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1853,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4848076B-E6B2-4A92-8D92-BEA8639DFA70}">
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -1869,502 +1929,502 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="R1" s="15" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="R1" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+      <c r="Y1" s="43"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="42"/>
+      <c r="E2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="42"/>
+      <c r="M2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="42"/>
+      <c r="O2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="R2" s="11"/>
+      <c r="P2" s="42"/>
+      <c r="R2" s="1"/>
       <c r="S2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8" t="s">
+      <c r="U2" s="42"/>
+      <c r="V2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8" t="s">
+      <c r="W2" s="42"/>
+      <c r="X2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="8"/>
+      <c r="Y2" s="42"/>
     </row>
     <row r="3" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="V3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="W3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y3" s="24" t="s">
+      <c r="C3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="21">
         <v>3.5331000000000001</v>
       </c>
-      <c r="D4" s="49">
+      <c r="D4" s="36">
         <v>6.0150000000000002E-2</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="22">
         <v>10.601699999999999</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="22">
         <v>1.1299999999999999E-3</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="21">
         <v>2.81E-2</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="21">
         <v>0.86687999999999998</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="21">
         <v>2.3E-2</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="21">
         <v>0.87939000000000001</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="22">
         <v>6.4859</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="22">
         <v>1.0869999999999999E-2</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="21">
         <v>1.016</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="21">
         <v>0.31347999999999998</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="21">
         <v>2.2452999999999999</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="21">
         <v>0.13402</v>
       </c>
-      <c r="R4" s="11"/>
+      <c r="R4" s="1"/>
       <c r="S4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="5">
         <v>15.289199999999999</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="7">
+      <c r="V4" s="5">
         <v>13.670500000000001</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="W4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="6">
+      <c r="X4" s="4">
         <v>1.6815</v>
       </c>
-      <c r="Y4" s="6">
+      <c r="Y4" s="4">
         <v>0.1947208</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="21">
         <v>2.7665999999999999</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="36">
         <v>9.6250000000000002E-2</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="21">
         <v>1.2419</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="21">
         <v>0.26511000000000001</v>
       </c>
-      <c r="G5" s="30">
+      <c r="G5" s="21">
         <v>0.52829999999999999</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="21">
         <v>0.46732000000000001</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="21">
         <v>0.2878</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="21">
         <v>0.59162999999999999</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="21">
         <v>2.6844999999999999</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="21">
         <v>0.10133</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="21">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="23">
         <v>0.89363000000000004</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="22">
         <v>5.0782999999999996</v>
       </c>
-      <c r="P5" s="48">
+      <c r="P5" s="35">
         <v>2.4230000000000002E-2</v>
       </c>
-      <c r="R5" s="11"/>
+      <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="5">
         <v>9.0170999999999992</v>
       </c>
-      <c r="U5" s="7">
+      <c r="U5" s="5">
         <v>2.6749999999999999E-3</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="4">
         <v>2.2999000000000001</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="4">
         <v>0.12937899999999999</v>
       </c>
-      <c r="X5" s="6">
+      <c r="X5" s="4">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="Y5" s="12">
         <v>0.937662</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="22">
         <v>5.9622000000000002</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="22">
         <v>1.4619999999999999E-2</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="22">
         <v>8.7955000000000005</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="34">
+      <c r="G6" s="21">
         <v>3.1099999999999999E-2</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="21">
         <v>0.86009999999999998</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="21">
         <v>0.37430000000000002</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="21">
         <v>0.54069</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="21">
         <v>1.4116</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="21">
         <v>0.23479</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="21">
         <v>0.39500000000000002</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="21">
         <v>0.52968000000000004</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="22">
         <v>6.5929000000000002</v>
       </c>
-      <c r="P6" s="31">
+      <c r="P6" s="22">
         <v>1.0240000000000001E-2</v>
       </c>
-      <c r="R6" s="11"/>
+      <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="5">
         <v>33.511600000000001</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="U6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="5">
         <v>9.9451000000000001</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="5">
         <v>1.6130000000000001E-3</v>
       </c>
-      <c r="X6" s="6">
+      <c r="X6" s="4">
         <v>0.19139999999999999</v>
       </c>
-      <c r="Y6" s="6">
+      <c r="Y6" s="4">
         <v>0.66178099999999995</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="26">
         <v>0.16750000000000001</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="26">
         <v>0.68235999999999997</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="26">
         <v>2.7307000000000001</v>
       </c>
-      <c r="F7" s="50">
+      <c r="F7" s="37">
         <v>9.8430000000000004E-2</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="26">
         <v>0.20030000000000001</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="26">
         <v>0.65444999999999998</v>
       </c>
-      <c r="I7" s="36">
+      <c r="I7" s="26">
         <v>0.80740000000000001</v>
       </c>
-      <c r="J7" s="36">
+      <c r="J7" s="26">
         <v>0.36890000000000001</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="26">
         <v>1.5363</v>
       </c>
-      <c r="L7" s="36">
+      <c r="L7" s="26">
         <v>0.21517</v>
       </c>
-      <c r="M7" s="36">
+      <c r="M7" s="26">
         <v>2.35E-2</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="26">
         <v>0.87814000000000003</v>
       </c>
-      <c r="O7" s="36">
+      <c r="O7" s="26">
         <v>1.0640000000000001</v>
       </c>
-      <c r="P7" s="36">
+      <c r="P7" s="26">
         <v>0.30231000000000002</v>
       </c>
-      <c r="R7" s="11"/>
-      <c r="S7" s="19" t="s">
+      <c r="R7" s="1"/>
+      <c r="S7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="51">
+      <c r="T7" s="38">
         <v>0.5776</v>
       </c>
-      <c r="U7" s="22">
+      <c r="U7" s="13">
         <v>0.44724000000000003</v>
       </c>
-      <c r="V7" s="22">
+      <c r="V7" s="13">
         <v>3.6738</v>
       </c>
-      <c r="W7" s="22">
+      <c r="W7" s="13">
         <v>5.5280000000000003E-2</v>
       </c>
-      <c r="X7" s="22">
+      <c r="X7" s="13">
         <v>1.3526</v>
       </c>
-      <c r="Y7" s="22">
+      <c r="Y7" s="13">
         <v>0.24482999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="18">
         <v>1.4319999999999999</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="18">
         <v>0.23144400000000001</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="19">
         <v>8.5736000000000008</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="19">
         <v>3.411E-3</v>
       </c>
-      <c r="G8" s="27">
-        <v>0</v>
-      </c>
-      <c r="H8" s="27">
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
+      <c r="H8" s="18">
         <v>0.99728499999999998</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="40">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="J8" s="54">
+      <c r="J8" s="40">
         <v>0.78119700000000003</v>
       </c>
-      <c r="K8" s="55">
+      <c r="K8" s="41">
         <v>4.7351000000000001</v>
       </c>
-      <c r="L8" s="55">
+      <c r="L8" s="41">
         <v>2.9552999999999999E-2</v>
       </c>
-      <c r="M8" s="54">
+      <c r="M8" s="40">
         <v>1.1627000000000001</v>
       </c>
-      <c r="N8" s="54">
+      <c r="N8" s="40">
         <v>0.28090900000000002</v>
       </c>
-      <c r="O8" s="56">
+      <c r="O8" s="41">
         <v>3.8925000000000001</v>
       </c>
-      <c r="P8" s="55">
+      <c r="P8" s="41">
         <v>4.8502000000000003E-2</v>
       </c>
-      <c r="R8" s="11"/>
-      <c r="S8" s="20" t="s">
+      <c r="R8" s="1"/>
+      <c r="S8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="26">
+      <c r="T8" s="17">
         <v>12.452999999999999</v>
       </c>
-      <c r="U8" s="26" t="s">
+      <c r="U8" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="11">
         <v>10.601599999999999</v>
       </c>
-      <c r="W8" s="20">
+      <c r="W8" s="11">
         <v>1E-3</v>
       </c>
-      <c r="X8" s="20">
+      <c r="X8" s="11">
         <v>0.69040000000000001</v>
       </c>
-      <c r="Y8" s="53">
+      <c r="Y8" s="39">
         <v>0.40600000000000003</v>
       </c>
     </row>
@@ -2386,4 +2446,337 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB648CF1-065B-4797-AD68-79CA2A54755A}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+    </row>
+    <row r="2" spans="1:8" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="E4" s="5">
+        <v>31.510999999999999</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5">
+        <v>10.340999999999999</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2.415</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.12</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.182</v>
+      </c>
+      <c r="G5" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.94799999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5.1680000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.3339999999999996</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="46">
+        <v>3.6789999999999998</v>
+      </c>
+      <c r="D7" s="47">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1.0201</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.312</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="48">
+        <v>5.57</v>
+      </c>
+      <c r="H8" s="14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="47">
+        <v>3.718</v>
+      </c>
+      <c r="D9" s="47">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5.8710000000000004</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+    </row>
+    <row r="11" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="50">
+        <v>2.44</v>
+      </c>
+      <c r="D11" s="49">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E11" s="51">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="F11" s="15">
+        <v>2E-3</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="42"/>
+    </row>
+    <row r="14" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="19">
+        <v>157.14699999999999</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="19">
+        <v>9.4529999999999994</v>
+      </c>
+      <c r="F15" s="19">
+        <v>2E-3</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A10:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Apdated analysis includes bioclimate variables. Shows an interesint pattern. Seasonality seems to explain the effect better than anything else.
</commit_message>
<xml_diff>
--- a/Output/Anova tables mericarp bioclimate.xlsx
+++ b/Output/Anova tables mericarp bioclimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Vault of Ideas\20 - 29 Tribulus Research\22 Chapter. Tribulus phenotypic variation in mainland and island populations\22.03 R code\Tribulus-mericarp-morphology\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF191A6-49B6-4464-AE0E-1C76F6AE2430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1104EF71-ECB4-4A63-B15E-B1E5ACFA1827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
+    <workbookView xWindow="10440" yWindow="360" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{B0106D92-7393-43C6-BB38-A2AE16D3AB1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual dataset" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="30">
   <si>
     <t>P</t>
   </si>
@@ -255,6 +255,38 @@
       <t>Galápagos removed</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A) Mericarp – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island - Galápagos removed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">B) Flowers – </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>continental vs island - Galápagos removed</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -498,35 +530,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC27BD51-B649-4FE2-8231-40ED64EB6F14}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:Y17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -860,84 +892,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="R1" s="43" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="R1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42" t="s">
+      <c r="N2" s="49"/>
+      <c r="O2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="42"/>
+      <c r="P2" s="49"/>
       <c r="R2" s="1"/>
       <c r="S2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="42" t="s">
+      <c r="T2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42" t="s">
+      <c r="U2" s="49"/>
+      <c r="V2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42" t="s">
+      <c r="W2" s="49"/>
+      <c r="X2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="42"/>
+      <c r="Y2" s="49"/>
     </row>
     <row r="3" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1430,82 +1462,82 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="R10" s="43" t="s">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="R10" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="43"/>
-      <c r="V10" s="43"/>
-      <c r="W10" s="43"/>
-      <c r="X10" s="43"/>
-      <c r="Y10" s="43"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="50"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42" t="s">
+      <c r="D11" s="49"/>
+      <c r="E11" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42" t="s">
+      <c r="F11" s="49"/>
+      <c r="G11" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42" t="s">
+      <c r="H11" s="49"/>
+      <c r="I11" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42" t="s">
+      <c r="J11" s="49"/>
+      <c r="K11" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42" t="s">
+      <c r="L11" s="49"/>
+      <c r="M11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42" t="s">
+      <c r="N11" s="49"/>
+      <c r="O11" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="42"/>
+      <c r="P11" s="49"/>
       <c r="R11" s="2"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="42" t="s">
+      <c r="T11" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="U11" s="42"/>
-      <c r="V11" s="42" t="s">
+      <c r="U11" s="49"/>
+      <c r="V11" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="W11" s="42"/>
-      <c r="X11" s="42" t="s">
+      <c r="W11" s="49"/>
+      <c r="X11" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="Y11" s="42"/>
+      <c r="Y11" s="49"/>
     </row>
     <row r="12" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -1644,82 +1676,82 @@
       </c>
     </row>
     <row r="14" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="R14" s="43" t="s">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="R14" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="S14" s="43"/>
-      <c r="T14" s="43"/>
-      <c r="U14" s="43"/>
-      <c r="V14" s="43"/>
-      <c r="W14" s="43"/>
-      <c r="X14" s="43"/>
-      <c r="Y14" s="43"/>
+      <c r="S14" s="50"/>
+      <c r="T14" s="50"/>
+      <c r="U14" s="50"/>
+      <c r="V14" s="50"/>
+      <c r="W14" s="50"/>
+      <c r="X14" s="50"/>
+      <c r="Y14" s="50"/>
     </row>
     <row r="15" spans="1:25" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44" t="s">
+      <c r="D15" s="48"/>
+      <c r="E15" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44" t="s">
+      <c r="F15" s="48"/>
+      <c r="G15" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44" t="s">
+      <c r="H15" s="48"/>
+      <c r="I15" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="44"/>
-      <c r="K15" s="44" t="s">
+      <c r="J15" s="48"/>
+      <c r="K15" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="44"/>
-      <c r="M15" s="44" t="s">
+      <c r="L15" s="48"/>
+      <c r="M15" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="44"/>
-      <c r="O15" s="44" t="s">
+      <c r="N15" s="48"/>
+      <c r="O15" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="44"/>
+      <c r="P15" s="48"/>
       <c r="R15" s="2"/>
       <c r="S15" s="5"/>
-      <c r="T15" s="42" t="s">
+      <c r="T15" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="42"/>
-      <c r="V15" s="42" t="s">
+      <c r="U15" s="49"/>
+      <c r="V15" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="W15" s="42"/>
-      <c r="X15" s="42" t="s">
+      <c r="W15" s="49"/>
+      <c r="X15" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="Y15" s="42"/>
+      <c r="Y15" s="49"/>
     </row>
     <row r="16" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -1867,30 +1899,6 @@
     <row r="34" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="A14:P14"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="A10:P10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="I15:J15"/>
     <mergeCell ref="T15:U15"/>
     <mergeCell ref="X15:Y15"/>
     <mergeCell ref="R1:Y1"/>
@@ -1903,6 +1911,30 @@
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="X11:Y11"/>
     <mergeCell ref="T2:U2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A10:P10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="A14:P14"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1929,84 +1961,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="R1" s="43" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="R1" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42" t="s">
+      <c r="H2" s="49"/>
+      <c r="I2" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42" t="s">
+      <c r="J2" s="49"/>
+      <c r="K2" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42" t="s">
+      <c r="L2" s="49"/>
+      <c r="M2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42" t="s">
+      <c r="N2" s="49"/>
+      <c r="O2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="42"/>
+      <c r="P2" s="49"/>
       <c r="R2" s="1"/>
       <c r="S2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="42" t="s">
+      <c r="T2" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42" t="s">
+      <c r="U2" s="49"/>
+      <c r="V2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42" t="s">
+      <c r="W2" s="49"/>
+      <c r="X2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="42"/>
+      <c r="Y2" s="49"/>
     </row>
     <row r="3" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2450,45 +2482,98 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB648CF1-065B-4797-AD68-79CA2A54755A}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-    </row>
-    <row r="2" spans="1:8" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="J1" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+    </row>
+    <row r="2" spans="1:25" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="49"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="49"/>
+    </row>
+    <row r="3" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="9"/>
       <c r="C3" s="15" t="s">
@@ -2509,17 +2594,65 @@
       <c r="H3" s="15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>7.4999999999999997E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="D4" s="4">
-        <v>0.78400000000000003</v>
+        <v>0.78700000000000003</v>
       </c>
       <c r="E4" s="5">
         <v>31.510999999999999</v>
@@ -2533,89 +2666,273 @@
       <c r="H4" s="5">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="21">
+        <v>1.6E-2</v>
+      </c>
+      <c r="M4" s="21">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="N4" s="22">
+        <v>17.491</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="21">
+        <v>0.871</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>0.35</v>
+      </c>
+      <c r="R4" s="21">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="S4" s="21">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="T4" s="22">
+        <v>3.4529999999999998</v>
+      </c>
+      <c r="U4" s="22">
+        <v>6.3E-2</v>
+      </c>
+      <c r="V4" s="21">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="W4" s="21">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="X4" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="Y4" s="21">
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>2.415</v>
+        <v>2.7949999999999999</v>
       </c>
       <c r="D5" s="12">
-        <v>0.12</v>
+        <v>9.4E-2</v>
       </c>
       <c r="E5" s="4">
-        <v>1.7749999999999999</v>
+        <v>0.99099999999999999</v>
       </c>
       <c r="F5" s="4">
-        <v>0.182</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="G5" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H5" s="12">
-        <v>0.94799999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="M5" s="21">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="N5" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="O5" s="21">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="P5" s="21">
+        <v>1.462</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>1.462</v>
+      </c>
+      <c r="R5" s="21">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="S5" s="21">
+        <v>0.82899999999999996</v>
+      </c>
+      <c r="T5" s="22">
+        <v>4.1989999999999998</v>
+      </c>
+      <c r="U5" s="35">
+        <v>0.04</v>
+      </c>
+      <c r="V5" s="22">
+        <v>4.3159999999999998</v>
+      </c>
+      <c r="W5" s="35">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="X5" s="21">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>0.78700000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>5.1680000000000001</v>
+        <v>5.843</v>
       </c>
       <c r="D6" s="5">
-        <v>2.3E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E6" s="5">
-        <v>6.3339999999999996</v>
+        <v>5.6619999999999999</v>
       </c>
       <c r="F6" s="5">
-        <v>1.0999999999999999E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G6" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H6" s="12">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="21">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="M6" s="23">
+        <v>0.19</v>
+      </c>
+      <c r="N6" s="21">
+        <v>1.446</v>
+      </c>
+      <c r="O6" s="23">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="P6" s="21">
+        <v>0.313</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="R6" s="21">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="S6" s="21">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="T6" s="22">
+        <v>3.891</v>
+      </c>
+      <c r="U6" s="22">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="V6" s="21">
+        <v>3.0270000000000001</v>
+      </c>
+      <c r="W6" s="21">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="X6" s="22">
+        <v>6.7169999999999996</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="46">
-        <v>3.6789999999999998</v>
-      </c>
-      <c r="D7" s="47">
-        <v>5.5E-2</v>
+      <c r="C7" s="16">
+        <v>4.5910000000000002</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E7" s="4">
-        <v>4.1000000000000002E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="F7" s="4">
-        <v>0.83799999999999997</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="G7" s="4">
-        <v>0.23499999999999999</v>
+        <v>2E-3</v>
       </c>
       <c r="H7" s="4">
-        <v>0.627</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="36">
+        <v>2.9929999999999999</v>
+      </c>
+      <c r="M7" s="51">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N7" s="21">
+        <v>1.429</v>
+      </c>
+      <c r="O7" s="21">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="P7" s="21">
+        <v>2.5009999999999999</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>0.113</v>
+      </c>
+      <c r="R7" s="21">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="S7" s="21">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="T7" s="22">
+        <v>4.7670000000000003</v>
+      </c>
+      <c r="U7" s="22">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="V7" s="22">
+        <v>18.585000000000001</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="X7" s="22">
+        <v>8.5980000000000008</v>
+      </c>
+      <c r="Y7" s="22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="13">
-        <v>1.0201</v>
+        <v>1.3420000000000001</v>
       </c>
       <c r="D8" s="13">
-        <v>0.312</v>
+        <v>0.246</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>22</v>
@@ -2623,153 +2940,327 @@
       <c r="F8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="48">
-        <v>5.57</v>
-      </c>
-      <c r="H8" s="14">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="G8" s="44">
+        <v>5.3639999999999999</v>
+      </c>
+      <c r="H8" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="25">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="M8" s="26">
+        <v>0.435</v>
+      </c>
+      <c r="N8" s="26">
+        <v>0</v>
+      </c>
+      <c r="O8" s="26">
+        <v>0.999</v>
+      </c>
+      <c r="P8" s="26">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="Q8" s="25">
+        <v>0.309</v>
+      </c>
+      <c r="R8" s="26">
+        <v>1.115</v>
+      </c>
+      <c r="S8" s="25">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="T8" s="26">
+        <v>2.7E-2</v>
+      </c>
+      <c r="U8" s="26">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="V8" s="26">
+        <v>1.9910000000000001</v>
+      </c>
+      <c r="W8" s="13">
+        <v>0.158</v>
+      </c>
+      <c r="X8" s="27">
+        <v>6.9059999999999997</v>
+      </c>
+      <c r="Y8" s="14">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="47">
-        <v>3.718</v>
-      </c>
-      <c r="D9" s="47">
-        <v>5.2999999999999999E-2</v>
+      <c r="C9" s="43">
+        <v>3.2519999999999998</v>
+      </c>
+      <c r="D9" s="43">
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E9" s="5">
-        <v>5.8710000000000004</v>
+        <v>6.0540000000000003</v>
       </c>
       <c r="F9" s="5">
-        <v>1.4999999999999999E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="G9" s="4">
-        <v>0.13100000000000001</v>
+        <v>0.52600000000000002</v>
       </c>
       <c r="H9" s="4">
-        <v>0.71599999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="4">
+        <v>1.022</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.311</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="O9" s="4">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="P9" s="4">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="R9" s="21">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="S9" s="21">
+        <v>0.629</v>
+      </c>
+      <c r="T9" s="22">
+        <v>6.0090000000000003</v>
+      </c>
+      <c r="U9" s="22">
+        <v>1.4E-2</v>
+      </c>
+      <c r="V9" s="22">
+        <v>9.032</v>
+      </c>
+      <c r="W9" s="22">
+        <v>2E-3</v>
+      </c>
+      <c r="X9" s="21">
+        <v>0.128</v>
+      </c>
+      <c r="Y9" s="21">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-    </row>
-    <row r="11" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="J10" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+    </row>
+    <row r="11" spans="1:25" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="50">
+      <c r="C11" s="46">
         <v>2.44</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="45">
         <v>0.11799999999999999</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="47">
         <v>9.0399999999999991</v>
       </c>
       <c r="F11" s="15">
         <v>2E-3</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="49" t="s">
+      <c r="H11" s="45" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42" t="s">
+      <c r="J11" s="3"/>
+      <c r="K11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42" t="s">
+      <c r="O11" s="49"/>
+      <c r="P11" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="42"/>
-    </row>
-    <row r="14" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="18" t="s">
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y11" s="49"/>
+    </row>
+    <row r="12" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="3"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="19">
-        <v>157.14699999999999</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="19">
-        <v>9.4529999999999994</v>
-      </c>
-      <c r="F15" s="19">
-        <v>2E-3</v>
-      </c>
-      <c r="G15" s="18" t="s">
+      <c r="L13" s="30">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M13" s="30">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="N13" s="29">
+        <v>7.88</v>
+      </c>
+      <c r="O13" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="Q13" s="21" t="s">
         <v>22</v>
       </c>
+      <c r="R13" s="28">
+        <v>4.7809999999999997</v>
+      </c>
+      <c r="S13" s="5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="T13" s="28">
+        <v>8.1489999999999991</v>
+      </c>
+      <c r="U13" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="V13" s="30">
+        <v>1.353</v>
+      </c>
+      <c r="W13" s="31">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="X13" s="29">
+        <v>7.63</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
+  <mergeCells count="21">
+    <mergeCell ref="J10:Y10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="T11:U11"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="J1:Y1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="X2:Y2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>

</xml_diff>